<commit_message>
Refactor onboarding and layout components for improved readability and functionality.
</commit_message>
<xml_diff>
--- a/src/lib/scripts/seed-data/production/targets.xlsx
+++ b/src/lib/scripts/seed-data/production/targets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93F730F-21FC-124B-AA76-8B2D949FA091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD9DFEC-B1F4-FA4A-8388-C2F98874C1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,57 +64,471 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Possible values:
-- B2B SaaS
-- Fintech
-- Healthtech
-- AI/ML
-- Deep tech
-- Climate tech
-- Consumer
-- E-commerce
-- Marketplace
-- Gaming
-- Web3
-- Developer tools
-- Cybersecurity
-- Logistics
-- AdTech
-- PropTech
-- InsurTech
-- Agriculture
-- Automotive
-- Biotechnology
-- Construction
-- Consulting
-- Consumer Goods
-- Education
-- Energy
-- Entertainment
-- Environmental Services
-- Fashion
-- Food &amp; Beverage
-- Government
-- Healthcare Services
-- Hospitality
-- Human Resources
-- Insurance
-- Legal
-- Manufacturing
-- Media
-- Non-profit
-- Pharmaceuticals
-- Real Estate
-- Retail
-- Telecommunications
-- Transportation
-- Utilities
-- Other</t>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Possible values:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- B2B SaaS
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Fintech
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Healthtech
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- AI/ML
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Deep tech
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Climate tech
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Consumer
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- E-commerce
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Marketplace
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Gaming
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Web3
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Developer tools
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Cybersecurity
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Logistics
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- AdTech
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- PropTech
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- InsurTech
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Agriculture
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Automotive
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Biotechnology
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Construction
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Consulting
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Consumer Goods
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Education
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Energy
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Entertainment
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Environmental Services
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Fashion
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Food &amp; Beverage
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Government
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Healthcare Services
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Hospitality
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Human Resources
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Insurance
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Legal
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Manufacturing
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Media
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Non-profit
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Pharmaceuticals
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Real Estate
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Retail
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Telecommunications
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Transportation
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Utilities
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>- Other</t>
         </r>
       </text>
     </comment>
@@ -123,29 +537,191 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Possible values:
-- Global
-- North America
-- South America
-- LATAM
-- Europe
-- Western Europe
-- Eastern Europe
-- Continental Europe
-- Middle East
-- Africa
-- Asia
-- East Asia
-- South Asia
-- South East Asia
-- Oceania
-- EMEA
-- Emerging Markets</t>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Possible values:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Global
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- North America
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- South America
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- LATAM
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Europe
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Western Europe
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Eastern Europe
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Continental Europe
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Middle East
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Africa
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Asia
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- East Asia
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- South Asia
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- South East Asia
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- Oceania
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- EMEA
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>- Emerging Markets</t>
         </r>
       </text>
     </comment>
@@ -225,7 +801,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="113">
   <si>
     <t>name</t>
   </si>
@@ -540,13 +1116,37 @@
   </si>
   <si>
     <t>It is the v0 app</t>
+  </si>
+  <si>
+    <t>Breega</t>
+  </si>
+  <si>
+    <t>https://www.breega.com/</t>
+  </si>
+  <si>
+    <t>https://rm531z4dws8.typeform.com/to/NNZmuM7H?typeform-source=www.breega.com</t>
+  </si>
+  <si>
+    <t>B2B SaaS, Fintech, Consumer</t>
+  </si>
+  <si>
+    <t>EMEA, Emerging Markets</t>
+  </si>
+  <si>
+    <t>pitch_deck, video</t>
+  </si>
+  <si>
+    <t>we back exceptional founders—sometimes before they even see it themselves—from pre-Seed to Series A+, building Digital, Climate, and Deep Tech startups ...</t>
+  </si>
+  <si>
+    <t>Pre-seed; Pre-seed; Series A; Series B; Growth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,6 +1179,12 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -972,28 +1578,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BM2"/>
+  <dimension ref="A1:BM3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="54.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="65" width="8.83203125" style="7"/>
     <col min="66" max="16384" width="8.83203125" style="5"/>
   </cols>
@@ -1121,8 +1728,8 @@
       <c r="J2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>28</v>
+      <c r="K2" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>101</v>
@@ -1185,6 +1792,47 @@
       <c r="BL2" s="4"/>
       <c r="BM2" s="4"/>
     </row>
+    <row r="3" spans="1:65" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{3EED2346-1F23-9440-9F28-4BC2E28B4743}"/>
@@ -1236,7 +1884,7 @@
           <x14:formula1>
             <xm:f>ValidationData!$K$1:$K$5</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K1000</xm:sqref>
+          <xm:sqref>K2:K1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-00000E000000}">
           <x14:formula1>

</xml_diff>

<commit_message>
Enhance submission handling in dashboard components by integrating job status checks from Hyperbrowser API, improving error handling, and adding column visibility options in applications table.
</commit_message>
<xml_diff>
--- a/src/lib/scripts/seed-data/production/targets.xlsx
+++ b/src/lib/scripts/seed-data/production/targets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD9DFEC-B1F4-FA4A-8388-C2F98874C1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0937CD-2E67-D946-B0F1-AFDF9E2277EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1139,7 +1139,7 @@
     <t>we back exceptional founders—sometimes before they even see it themselves—from pre-Seed to Series A+, building Digital, Climate, and Deep Tech startups ...</t>
   </si>
   <si>
-    <t>Pre-seed; Pre-seed; Series A; Series B; Growth</t>
+    <t>Pre-seed; Series A; Series B; Growth</t>
   </si>
 </sst>
 </file>
@@ -1582,7 +1582,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>